<commit_message>
Módulo 12 - Finalização do módulo
</commit_message>
<xml_diff>
--- a/Módulo 12/aula-grava-macro.xlsx
+++ b/Módulo 12/aula-grava-macro.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FichaMatriz" sheetId="3" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>CONTROLE DE ALMOXARIFADO</t>
   </si>
@@ -56,7 +57,41 @@
     <t>QUANTIDADE</t>
   </si>
   <si>
-    <t>Macro é utilizado para automatizar tarefas repetitivas.Guia desenvolvedor: arquivo/opções/personalizar faixas de opções/aba guias principais/ desenvolvedor</t>
+    <t>Macro é utilizado para automatizar tarefas repetitivas.Guia desenvolvedor: arquivo/opções/personalizar faixas de opções/aba guias principais/ desenvolvedor
+Gravar uma macro: na fig no rodapé esquerdo ou aba exibição/Macros/gravar macros ou aba desenvolvedor/gravar macro.Dá o nome da macro sem espaços, coloca uma descrição se quiser/ok a macro já começa a ser gravada, com isso pode fazer os passos que deseja, tudo que vc fizer será gravado com exceção do movimento do mouse. A ação feita neste exemplo foi a criação de uma nova ficha. Ao final basta parar a gravação.
+Para atribuir uma gravação de macro para um botão basta clicar como o botão direito em cima do elemento/pressionar a opção atribuir macro/selecionar a macro e clicar em ok.
+Para que uma macro funcionar em todas as planilhas criadas, eu não posso ter atrelado á planilha um nome de tabelas diferente, ou seja, todas as tabelas devem ter o mesmo nome.</t>
+  </si>
+  <si>
+    <t>1° Tranforma atabela em um
+ intervalo de dados.
+Clica na tabela/converter em
+intervalo de dados.
+Para selecionar uma coluna inteira basta inserir a letra da coluna/dois pontos letra da coluna novamente</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -130,7 +165,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +190,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -252,11 +311,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -264,9 +334,6 @@
     <xf numFmtId="14" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -305,9 +372,6 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -340,6 +404,20 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -354,114 +432,24 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -489,12 +477,12 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="[0]!Duplica" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo: Cantos Arredondados 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00C46181-E0CD-476E-99E6-FFF30C882F09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00C46181-E0CD-476E-99E6-FFF30C882F09}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -566,7 +554,7 @@
         <xdr:cNvPr id="4" name="Retângulo: Cantos Arredondados 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2FD5F-3043-4017-8802-6355E0E4FA81}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2FD5F-3043-4017-8802-6355E0E4FA81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -638,7 +626,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Arredondados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A0BBA5-5516-46B4-A9A9-21CF4507C63D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{70A0BBA5-5516-46B4-A9A9-21CF4507C63D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -693,19 +681,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TBEstoques" displayName="TBEstoques" ref="G1:J2" insertRow="1" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="G1:J2"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="DATA" dataDxfId="3"/>
-    <tableColumn id="2" name="ENTRADA" dataDxfId="2"/>
-    <tableColumn id="3" name="SAÍDA" dataDxfId="1"/>
-    <tableColumn id="4" name="DESTINO" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1008,17 +983,17 @@
   <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:E17"/>
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="4" customWidth="1"/>
-    <col min="3" max="5" width="20.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="3" customWidth="1"/>
+    <col min="3" max="5" width="20.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="6" customWidth="1"/>
     <col min="8" max="9" width="15.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="29.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="5.7109375" style="1" customWidth="1"/>
@@ -1029,163 +1004,176 @@
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="9"/>
-      <c r="G1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="8"/>
+      <c r="G1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="27" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="18"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="G2" s="3">
+        <v>44022</v>
+      </c>
+      <c r="H2" s="6">
+        <v>30</v>
+      </c>
+      <c r="I2" s="6">
+        <v>10</v>
+      </c>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="30"/>
+      <c r="D4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="25">
-        <f>SUM(TBEstoques[ENTRADA])-SUM(TBEstoques[SAÍDA])</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="23">
+        <f>SUM(H:H)-SUM(I:I)</f>
+        <v>20</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="19">
+        <v>43863</v>
+      </c>
+      <c r="E8" s="20">
+        <v>10</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="17" spans="2:7" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="17" spans="2:7" s="25" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="33" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="34"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
-  <mergeCells count="3">
+  <sheetProtection selectLockedCells="1" autoFilter="0"/>
+  <mergeCells count="4">
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Destino Inválido!" error="Selecione uma das opções disponíveis." sqref="C12">
@@ -1198,8 +1186,85 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>